<commit_message>
update data add replacemant talent add random property
</commit_message>
<xml_diff>
--- a/data/achievement.xlsx
+++ b/data/achievement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84694\Desktop\人生重来\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D59C89D-35FE-42A2-BD5F-BEA51D64AC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192AAC15-664F-426D-8674-7964E8F2D586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="504">
   <si>
     <t>$id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1482,10 +1482,6 @@
   </si>
   <si>
     <t>信条</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EVT?[11468,11469]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -2024,10 +2020,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>(ATLT?[1023])&amp;(ATLT?[1048])&amp;(ATLT?[1064])&amp;(ATLT?[1114])&amp;(ATLT?[1135])</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>嫁衣</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -2053,6 +2045,38 @@
   </si>
   <si>
     <t>EVT?[40070]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EVT?[11468,11469,20390]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(ATLT?[1023])&amp;(ATLT?[1048])&amp;(ATLT?[1064])&amp;(ATLT?[1114])&amp;(ATLT?[1135])&amp;(ATLT?[1141])</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>有会员，所以急着投胎</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(TLT?[1122])&amp;(TLT?[1141])</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>薅羊毛专家</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上当了</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TLT?[1136]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>太贪婪而被骗</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2440,11 +2464,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M162"/>
+  <dimension ref="A1:M166"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E162" sqref="E162"/>
+      <pane ySplit="2" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.44140625" defaultRowHeight="19.2" x14ac:dyDescent="0.25"/>
@@ -2475,13 +2499,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -2501,13 +2525,13 @@
         <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -2534,7 +2558,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2542,7 +2566,7 @@
         <v>102</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>10</v>
@@ -2557,7 +2581,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2580,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2588,7 +2612,7 @@
         <v>104</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
@@ -2603,7 +2627,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2620,13 +2644,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F7" s="5">
         <v>0</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2643,13 +2667,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2666,13 +2690,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F9" s="5">
         <v>0</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2689,13 +2713,13 @@
         <v>3</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F10" s="5">
         <v>1</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2712,13 +2736,13 @@
         <v>3</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F11" s="5">
         <v>1</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2741,7 +2765,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2758,13 +2782,13 @@
         <v>2</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F13" s="5">
         <v>1</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2787,7 +2811,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2810,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2833,7 +2857,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2856,7 +2880,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2873,13 +2897,13 @@
         <v>0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F18" s="5">
         <v>0</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2896,13 +2920,13 @@
         <v>0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F19" s="5">
         <v>0</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2919,13 +2943,13 @@
         <v>0</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F20" s="5">
         <v>0</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2942,13 +2966,13 @@
         <v>0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F21" s="5">
         <v>0</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2965,13 +2989,13 @@
         <v>0</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F22" s="5">
         <v>0</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2988,13 +3012,13 @@
         <v>1</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F23" s="5">
         <v>0</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3011,13 +3035,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F24" s="5">
         <v>0</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3034,13 +3058,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F25" s="5">
         <v>0</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3057,13 +3081,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F26" s="5">
         <v>0</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3080,13 +3104,13 @@
         <v>1</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F27" s="5">
         <v>0</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3103,13 +3127,13 @@
         <v>3</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F28" s="5">
         <v>1</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3126,13 +3150,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F29" s="5">
         <v>0</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3149,13 +3173,13 @@
         <v>2</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F30" s="5">
         <v>0</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3172,13 +3196,13 @@
         <v>3</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F31" s="5">
         <v>1</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3201,7 +3225,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3224,7 +3248,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3247,7 +3271,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3270,7 +3294,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3293,7 +3317,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3316,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3339,7 +3363,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3362,7 +3386,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3385,7 +3409,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3408,7 +3432,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3431,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3454,7 +3478,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3477,7 +3501,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3500,7 +3524,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3523,7 +3547,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3546,7 +3570,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3569,7 +3593,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3592,7 +3616,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3615,7 +3639,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3638,7 +3662,7 @@
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3661,7 +3685,7 @@
         <v>0</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3684,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3707,7 +3731,7 @@
         <v>0</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3730,7 +3754,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3753,7 +3777,7 @@
         <v>0</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3770,13 +3794,13 @@
         <v>1</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F57" s="5">
         <v>0</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3799,7 +3823,7 @@
         <v>0</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3822,7 +3846,7 @@
         <v>0</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3839,13 +3863,13 @@
         <v>1</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F60" s="5">
         <v>1</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3868,7 +3892,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3885,13 +3909,13 @@
         <v>2</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F62" s="5">
         <v>1</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3914,7 +3938,7 @@
         <v>0</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3937,7 +3961,7 @@
         <v>0</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3960,7 +3984,7 @@
         <v>0</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3983,7 +4007,7 @@
         <v>0</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4006,7 +4030,7 @@
         <v>0</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4029,7 +4053,7 @@
         <v>1</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4052,7 +4076,7 @@
         <v>0</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4075,7 +4099,7 @@
         <v>0</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4098,7 +4122,7 @@
         <v>0</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4121,7 +4145,7 @@
         <v>0</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4144,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4167,7 +4191,7 @@
         <v>0</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4190,7 +4214,7 @@
         <v>0</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4213,7 +4237,7 @@
         <v>0</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4236,7 +4260,7 @@
         <v>0</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4259,7 +4283,7 @@
         <v>0</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4282,7 +4306,7 @@
         <v>0</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4305,7 +4329,7 @@
         <v>0</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4328,7 +4352,7 @@
         <v>0</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4351,7 +4375,7 @@
         <v>0</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4374,7 +4398,7 @@
         <v>0</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4397,7 +4421,7 @@
         <v>0</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4420,7 +4444,7 @@
         <v>0</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4443,7 +4467,7 @@
         <v>0</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4466,7 +4490,7 @@
         <v>0</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4489,7 +4513,7 @@
         <v>0</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4512,7 +4536,7 @@
         <v>0</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4535,7 +4559,7 @@
         <v>1</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4558,7 +4582,7 @@
         <v>0</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4581,7 +4605,7 @@
         <v>1</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4604,7 +4628,7 @@
         <v>1</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4627,7 +4651,7 @@
         <v>0</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4635,7 +4659,7 @@
         <v>193</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>258</v>
@@ -4650,7 +4674,7 @@
         <v>0</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4673,7 +4697,7 @@
         <v>0</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4696,7 +4720,7 @@
         <v>0</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4719,7 +4743,7 @@
         <v>0</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4742,7 +4766,7 @@
         <v>1</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4765,7 +4789,7 @@
         <v>1</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4788,7 +4812,7 @@
         <v>0</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4811,7 +4835,7 @@
         <v>0</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4834,7 +4858,7 @@
         <v>0</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4857,7 +4881,7 @@
         <v>0</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4880,7 +4904,7 @@
         <v>1</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4903,7 +4927,7 @@
         <v>0</v>
       </c>
       <c r="G106" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4926,7 +4950,7 @@
         <v>0</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4949,7 +4973,7 @@
         <v>0</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4972,7 +4996,7 @@
         <v>0</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4995,7 +5019,7 @@
         <v>0</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5018,7 +5042,7 @@
         <v>0</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5041,7 +5065,7 @@
         <v>0</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5064,7 +5088,7 @@
         <v>0</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5087,7 +5111,7 @@
         <v>0</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5110,7 +5134,7 @@
         <v>0</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5133,7 +5157,7 @@
         <v>0</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5156,7 +5180,7 @@
         <v>1</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5179,7 +5203,7 @@
         <v>0</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5202,7 +5226,7 @@
         <v>0</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5225,7 +5249,7 @@
         <v>0</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5242,13 +5266,13 @@
         <v>3</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F121" s="5">
         <v>0</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5271,7 +5295,7 @@
         <v>0</v>
       </c>
       <c r="G122" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5294,7 +5318,7 @@
         <v>0</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5317,7 +5341,7 @@
         <v>0</v>
       </c>
       <c r="G124" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5340,7 +5364,7 @@
         <v>0</v>
       </c>
       <c r="G125" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5363,7 +5387,7 @@
         <v>0</v>
       </c>
       <c r="G126" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5374,19 +5398,19 @@
         <v>355</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D127" s="5">
         <v>1</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>356</v>
+        <v>496</v>
       </c>
       <c r="F127" s="5">
         <v>0</v>
       </c>
       <c r="G127" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5394,22 +5418,22 @@
         <v>226</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D128" s="5">
         <v>2</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F128" s="5">
         <v>1</v>
       </c>
       <c r="G128" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5417,22 +5441,22 @@
         <v>227</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D129" s="5">
         <v>1</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F129" s="5">
         <v>1</v>
       </c>
       <c r="G129" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5440,22 +5464,22 @@
         <v>228</v>
       </c>
       <c r="B130" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="C130" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="C130" s="5" t="s">
-        <v>365</v>
-      </c>
       <c r="D130" s="5">
         <v>1</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F130" s="5">
         <v>0</v>
       </c>
       <c r="G130" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5463,22 +5487,22 @@
         <v>229</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D131" s="5">
         <v>2</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F131" s="5">
         <v>0</v>
       </c>
       <c r="G131" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5486,22 +5510,22 @@
         <v>230</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D132" s="5">
         <v>1</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F132" s="5">
         <v>0</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5509,22 +5533,22 @@
         <v>231</v>
       </c>
       <c r="B133" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="D133" s="5">
+        <v>0</v>
+      </c>
+      <c r="E133" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="C133" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="D133" s="5">
-        <v>0</v>
-      </c>
-      <c r="E133" s="5" t="s">
-        <v>377</v>
-      </c>
       <c r="F133" s="5">
         <v>0</v>
       </c>
       <c r="G133" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5532,22 +5556,22 @@
         <v>232</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D134" s="5">
         <v>0</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F134" s="5">
         <v>0</v>
       </c>
       <c r="G134" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5555,22 +5579,22 @@
         <v>233</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D135" s="5">
         <v>0</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F135" s="5">
         <v>0</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5578,22 +5602,22 @@
         <v>234</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D136" s="5">
         <v>0</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F136" s="5">
         <v>0</v>
       </c>
       <c r="G136" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5601,22 +5625,22 @@
         <v>235</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D137" s="5">
         <v>0</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F137" s="5">
         <v>0</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5624,22 +5648,22 @@
         <v>236</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D138" s="5">
         <v>0</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F138" s="5">
         <v>0</v>
       </c>
       <c r="G138" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5647,22 +5671,22 @@
         <v>237</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D139" s="5">
         <v>0</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F139" s="5">
         <v>0</v>
       </c>
       <c r="G139" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5670,22 +5694,22 @@
         <v>238</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D140" s="5">
         <v>1</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F140" s="5">
         <v>0</v>
       </c>
       <c r="G140" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5693,22 +5717,22 @@
         <v>239</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D141" s="5">
         <v>1</v>
       </c>
       <c r="E141" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F141" s="5">
         <v>0</v>
       </c>
       <c r="G141" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5716,22 +5740,22 @@
         <v>240</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D142" s="5">
         <v>1</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F142" s="5">
         <v>0</v>
       </c>
       <c r="G142" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5739,22 +5763,22 @@
         <v>241</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D143" s="5">
         <v>1</v>
       </c>
       <c r="E143" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F143" s="5">
         <v>0</v>
       </c>
       <c r="G143" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5762,22 +5786,22 @@
         <v>242</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D144" s="5">
         <v>1</v>
       </c>
       <c r="E144" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F144" s="5">
         <v>0</v>
       </c>
       <c r="G144" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5785,22 +5809,22 @@
         <v>243</v>
       </c>
       <c r="B145" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="D145" s="5">
+        <v>0</v>
+      </c>
+      <c r="E145" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="C145" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="D145" s="5">
-        <v>0</v>
-      </c>
-      <c r="E145" s="5" t="s">
-        <v>414</v>
-      </c>
       <c r="F145" s="5">
         <v>0</v>
       </c>
       <c r="G145" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5808,22 +5832,22 @@
         <v>244</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D146" s="5">
         <v>0</v>
       </c>
       <c r="E146" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F146" s="5">
         <v>0</v>
       </c>
       <c r="G146" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5831,22 +5855,22 @@
         <v>245</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D147" s="5">
         <v>0</v>
       </c>
       <c r="E147" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F147" s="5">
         <v>0</v>
       </c>
       <c r="G147" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5854,22 +5878,22 @@
         <v>246</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D148" s="5">
         <v>1</v>
       </c>
       <c r="E148" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F148" s="5">
         <v>0</v>
       </c>
       <c r="G148" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5877,22 +5901,22 @@
         <v>247</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D149" s="5">
         <v>2</v>
       </c>
       <c r="E149" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F149" s="5">
         <v>1</v>
       </c>
       <c r="G149" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5900,22 +5924,22 @@
         <v>248</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D150" s="5">
         <v>3</v>
       </c>
       <c r="E150" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F150" s="5">
         <v>1</v>
       </c>
       <c r="G150" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5923,22 +5947,22 @@
         <v>249</v>
       </c>
       <c r="B151" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C151" s="5" t="s">
         <v>455</v>
       </c>
-      <c r="C151" s="5" t="s">
-        <v>456</v>
-      </c>
       <c r="D151" s="5">
         <v>1</v>
       </c>
       <c r="E151" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F151" s="5">
         <v>1</v>
       </c>
       <c r="G151" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5946,22 +5970,22 @@
         <v>250</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D152" s="5">
         <v>1</v>
       </c>
       <c r="E152" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F152" s="5">
         <v>1</v>
       </c>
       <c r="G152" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5969,22 +5993,22 @@
         <v>251</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D153" s="5">
         <v>2</v>
       </c>
       <c r="E153" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F153" s="5">
         <v>1</v>
       </c>
       <c r="G153" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5992,22 +6016,22 @@
         <v>252</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D154" s="5">
         <v>2</v>
       </c>
       <c r="E154" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F154" s="5">
         <v>0</v>
       </c>
       <c r="G154" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6015,22 +6039,22 @@
         <v>253</v>
       </c>
       <c r="B155" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="C155" s="5" t="s">
         <v>472</v>
-      </c>
-      <c r="C155" s="5" t="s">
-        <v>473</v>
       </c>
       <c r="D155" s="5">
         <v>3</v>
       </c>
       <c r="E155" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F155" s="5">
         <v>1</v>
       </c>
       <c r="G155" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6038,22 +6062,22 @@
         <v>254</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D156" s="5">
         <v>2</v>
       </c>
       <c r="E156" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F156" s="5">
         <v>1</v>
       </c>
       <c r="G156" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6061,22 +6085,22 @@
         <v>255</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D157" s="5">
         <v>3</v>
       </c>
       <c r="E157" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F157" s="5">
         <v>1</v>
       </c>
       <c r="G157" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6084,22 +6108,22 @@
         <v>256</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D158" s="5">
         <v>3</v>
       </c>
       <c r="E158" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F158" s="5">
         <v>1</v>
       </c>
       <c r="G158" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6107,22 +6131,22 @@
         <v>257</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C159" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="D159" s="5">
+        <v>0</v>
+      </c>
+      <c r="E159" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="D159" s="5">
-        <v>0</v>
-      </c>
-      <c r="E159" s="5" t="s">
-        <v>485</v>
-      </c>
       <c r="F159" s="5">
         <v>0</v>
       </c>
       <c r="G159" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6130,22 +6154,22 @@
         <v>258</v>
       </c>
       <c r="B160" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="D160" s="5">
+        <v>1</v>
+      </c>
+      <c r="E160" s="5" t="s">
         <v>488</v>
       </c>
-      <c r="C160" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="D160" s="5">
-        <v>1</v>
-      </c>
-      <c r="E160" s="5" t="s">
-        <v>489</v>
-      </c>
       <c r="F160" s="5">
         <v>0</v>
       </c>
       <c r="G160" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6153,22 +6177,22 @@
         <v>259</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D161" s="5">
         <v>2</v>
       </c>
       <c r="E161" s="5" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F161" s="5">
         <v>1</v>
       </c>
       <c r="G161" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6176,23 +6200,75 @@
         <v>260</v>
       </c>
       <c r="B162" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="D162" s="5">
+        <v>1</v>
+      </c>
+      <c r="E162" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="C162" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="D162" s="5">
-        <v>1</v>
-      </c>
-      <c r="E162" s="5" t="s">
-        <v>497</v>
-      </c>
       <c r="F162" s="5">
         <v>1</v>
       </c>
       <c r="G162" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="5">
+        <v>261</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="D163" s="5">
+        <v>2</v>
+      </c>
+      <c r="E163" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="F163" s="5">
+        <v>0</v>
+      </c>
+      <c r="G163" s="5" t="s">
         <v>441</v>
       </c>
+    </row>
+    <row r="164" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="5">
+        <v>262</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="D164" s="5">
+        <v>0</v>
+      </c>
+      <c r="E164" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="F164" s="5">
+        <v>1</v>
+      </c>
+      <c r="G164" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E165" s="5"/>
+    </row>
+    <row r="166" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E166" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>